<commit_message>
Implementado biblioteca pywhatkit e melhoria na logica de envio de mensagens
</commit_message>
<xml_diff>
--- a/marca-consulta/arquivos/agenda.xlsx
+++ b/marca-consulta/arquivos/agenda.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\TI\Documents\Programacao\Projetos\PYTHON\marca-consulta\arquivos\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documentos\Programacao\Projetos\PYTHON\marca-consulta\marca-consulta\arquivos\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1112" uniqueCount="95">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1140" uniqueCount="105">
   <si>
     <t>SEGUNDA</t>
   </si>
@@ -313,17 +313,47 @@
     <t>SÁBADO 21h</t>
   </si>
   <si>
-    <t xml:space="preserve">Estagiario Teste </t>
-  </si>
-  <si>
-    <t>Paciente Teste (19)</t>
+    <t>F122gq64gja7wONGzCReGs</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tonhao </t>
+  </si>
+  <si>
+    <t>Estagiario teste</t>
+  </si>
+  <si>
+    <t>fatima</t>
+  </si>
+  <si>
+    <t>bernardo</t>
+  </si>
+  <si>
+    <t>toinha</t>
+  </si>
+  <si>
+    <t>claudio</t>
+  </si>
+  <si>
+    <t>tiago</t>
+  </si>
+  <si>
+    <t>paiva</t>
+  </si>
+  <si>
+    <t>ronildo</t>
+  </si>
+  <si>
+    <t>fabiola</t>
+  </si>
+  <si>
+    <t>lucas</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="14" x14ac:knownFonts="1">
+  <fonts count="15" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -405,6 +435,13 @@
       <sz val="18"/>
       <color theme="1"/>
       <name val="Arial Black"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="5">
@@ -521,7 +558,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="31">
+  <cellXfs count="32">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -588,6 +625,7 @@
     <xf numFmtId="0" fontId="11" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="13" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -920,7 +958,7 @@
   <dimension ref="A1:E822"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
+      <selection activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -933,13 +971,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="28" t="s">
+      <c r="A1" s="29" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="29"/>
-      <c r="C1" s="29"/>
-      <c r="D1" s="29"/>
-      <c r="E1" s="30"/>
+      <c r="B1" s="30"/>
+      <c r="C1" s="30"/>
+      <c r="D1" s="30"/>
+      <c r="E1" s="31"/>
     </row>
     <row r="2" spans="1:5" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="27" t="s">
@@ -969,92 +1007,146 @@
         <v>999999999</v>
       </c>
       <c r="D3" s="6" t="s">
+        <v>95</v>
+      </c>
+      <c r="E3" s="6" t="s">
         <v>93</v>
-      </c>
-      <c r="E3" s="3">
-        <v>999999999</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B4" s="4"/>
+      <c r="B4" s="4" t="s">
+        <v>96</v>
+      </c>
       <c r="C4" s="4"/>
-      <c r="D4" s="6"/>
-      <c r="E4" s="5"/>
+      <c r="D4" s="6" t="s">
+        <v>95</v>
+      </c>
+      <c r="E4" s="6" t="s">
+        <v>93</v>
+      </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B5" s="15"/>
+      <c r="B5" s="15" t="s">
+        <v>97</v>
+      </c>
       <c r="C5" s="15"/>
-      <c r="D5" s="9"/>
-      <c r="E5" s="6"/>
+      <c r="D5" s="9" t="s">
+        <v>95</v>
+      </c>
+      <c r="E5" s="6" t="s">
+        <v>93</v>
+      </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B6" s="7"/>
+      <c r="B6" s="7" t="s">
+        <v>98</v>
+      </c>
       <c r="C6" s="7"/>
-      <c r="D6" s="3"/>
-      <c r="E6" s="8"/>
+      <c r="D6" s="3" t="s">
+        <v>95</v>
+      </c>
+      <c r="E6" s="6" t="s">
+        <v>93</v>
+      </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="B7" s="7"/>
+      <c r="B7" s="7" t="s">
+        <v>99</v>
+      </c>
       <c r="C7" s="7"/>
-      <c r="D7" s="9"/>
-      <c r="E7" s="3"/>
+      <c r="D7" s="9" t="s">
+        <v>95</v>
+      </c>
+      <c r="E7" s="6" t="s">
+        <v>93</v>
+      </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="B8" s="4"/>
+      <c r="B8" s="4" t="s">
+        <v>100</v>
+      </c>
       <c r="C8" s="4"/>
-      <c r="D8" s="12"/>
-      <c r="E8" s="8"/>
+      <c r="D8" s="12" t="s">
+        <v>95</v>
+      </c>
+      <c r="E8" s="6" t="s">
+        <v>93</v>
+      </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="B9" s="4"/>
+      <c r="B9" s="4" t="s">
+        <v>101</v>
+      </c>
       <c r="C9" s="4"/>
-      <c r="D9" s="3"/>
-      <c r="E9" s="3"/>
+      <c r="D9" s="3" t="s">
+        <v>95</v>
+      </c>
+      <c r="E9" s="6" t="s">
+        <v>93</v>
+      </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="B10" s="4"/>
+      <c r="B10" s="4" t="s">
+        <v>102</v>
+      </c>
       <c r="C10" s="4"/>
-      <c r="D10" s="3"/>
-      <c r="E10" s="3"/>
+      <c r="D10" s="3" t="s">
+        <v>95</v>
+      </c>
+      <c r="E10" s="6" t="s">
+        <v>93</v>
+      </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="B11" s="7"/>
+      <c r="B11" s="7" t="s">
+        <v>103</v>
+      </c>
       <c r="C11" s="7"/>
-      <c r="D11" s="12"/>
-      <c r="E11" s="8"/>
+      <c r="D11" s="12" t="s">
+        <v>95</v>
+      </c>
+      <c r="E11" s="6" t="s">
+        <v>93</v>
+      </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="B12" s="9"/>
+      <c r="B12" s="9" t="s">
+        <v>104</v>
+      </c>
       <c r="C12" s="9"/>
-      <c r="D12" s="9"/>
-      <c r="E12" s="3"/>
+      <c r="D12" s="9" t="s">
+        <v>95</v>
+      </c>
+      <c r="E12" s="6" t="s">
+        <v>93</v>
+      </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" s="26" t="s">
@@ -1141,7 +1233,7 @@
         <v>13</v>
       </c>
       <c r="B21" s="21"/>
-      <c r="C21" s="21"/>
+      <c r="C21" s="28"/>
       <c r="D21" s="22"/>
       <c r="E21" s="8"/>
     </row>
@@ -2270,13 +2362,13 @@
       <c r="E137" s="3"/>
     </row>
     <row r="138" spans="1:5" ht="27" x14ac:dyDescent="0.25">
-      <c r="A138" s="28" t="s">
+      <c r="A138" s="29" t="s">
         <v>28</v>
       </c>
-      <c r="B138" s="29"/>
-      <c r="C138" s="29"/>
-      <c r="D138" s="29"/>
-      <c r="E138" s="30"/>
+      <c r="B138" s="30"/>
+      <c r="C138" s="30"/>
+      <c r="D138" s="30"/>
+      <c r="E138" s="31"/>
     </row>
     <row r="139" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A139" s="27" t="s">
@@ -3599,13 +3691,13 @@
       <c r="E274" s="3"/>
     </row>
     <row r="275" spans="1:5" ht="27" x14ac:dyDescent="0.25">
-      <c r="A275" s="28" t="s">
+      <c r="A275" s="29" t="s">
         <v>41</v>
       </c>
-      <c r="B275" s="29"/>
-      <c r="C275" s="29"/>
-      <c r="D275" s="29"/>
-      <c r="E275" s="30"/>
+      <c r="B275" s="30"/>
+      <c r="C275" s="30"/>
+      <c r="D275" s="30"/>
+      <c r="E275" s="31"/>
     </row>
     <row r="276" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A276" s="27" t="s">
@@ -4928,13 +5020,13 @@
       <c r="E411" s="3"/>
     </row>
     <row r="412" spans="1:5" ht="27" x14ac:dyDescent="0.25">
-      <c r="A412" s="28" t="s">
+      <c r="A412" s="29" t="s">
         <v>54</v>
       </c>
-      <c r="B412" s="29"/>
-      <c r="C412" s="29"/>
-      <c r="D412" s="29"/>
-      <c r="E412" s="30"/>
+      <c r="B412" s="30"/>
+      <c r="C412" s="30"/>
+      <c r="D412" s="30"/>
+      <c r="E412" s="31"/>
     </row>
     <row r="413" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A413" s="27" t="s">
@@ -6257,13 +6349,13 @@
       <c r="E548" s="3"/>
     </row>
     <row r="549" spans="1:5" ht="27" x14ac:dyDescent="0.25">
-      <c r="A549" s="28" t="s">
+      <c r="A549" s="29" t="s">
         <v>67</v>
       </c>
-      <c r="B549" s="29"/>
-      <c r="C549" s="29"/>
-      <c r="D549" s="29"/>
-      <c r="E549" s="30"/>
+      <c r="B549" s="30"/>
+      <c r="C549" s="30"/>
+      <c r="D549" s="30"/>
+      <c r="E549" s="31"/>
     </row>
     <row r="550" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A550" s="27" t="s">
@@ -7586,13 +7678,13 @@
       <c r="E685" s="3"/>
     </row>
     <row r="686" spans="1:5" ht="27" x14ac:dyDescent="0.25">
-      <c r="A686" s="28" t="s">
+      <c r="A686" s="29" t="s">
         <v>80</v>
       </c>
-      <c r="B686" s="29"/>
-      <c r="C686" s="29"/>
-      <c r="D686" s="29"/>
-      <c r="E686" s="30"/>
+      <c r="B686" s="30"/>
+      <c r="C686" s="30"/>
+      <c r="D686" s="30"/>
+      <c r="E686" s="31"/>
     </row>
     <row r="687" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A687" s="27" t="s">

</xml_diff>